<commit_message>
Add code for experiment 3, MASS for T4 using T1, T2, T3
</commit_message>
<xml_diff>
--- a/output/AMC-5topics-result.xlsx
+++ b/output/AMC-5topics-result.xlsx
@@ -1,20 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28209"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quanguet/Dropbox/Documents/Education/Research/MASS-project-Cham-Ngan-Hong/output/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="AMC_5" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>train</t>
   </si>
@@ -30,12 +43,15 @@
   <si>
     <t>F1</t>
   </si>
+  <si>
+    <t>AMC_5</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,6 +114,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -144,12 +165,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -176,14 +197,15 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -210,6 +232,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -385,14 +408,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -409,7 +437,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -426,10 +454,10 @@
         <v>0.4758269720101781</v>
       </c>
       <c r="F2">
-        <v>0.5297450424929179</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>0.52974504249291787</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -440,16 +468,16 @@
         <v>500</v>
       </c>
       <c r="D3">
-        <v>0.7032258064516129</v>
+        <v>0.70322580645161292</v>
       </c>
       <c r="E3">
-        <v>0.55470737913486</v>
+        <v>0.55470737913486001</v>
       </c>
       <c r="F3">
-        <v>0.620199146514936</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>0.62019914651493602</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -460,16 +488,16 @@
         <v>600</v>
       </c>
       <c r="D4">
-        <v>0.7955974842767296</v>
+        <v>0.79559748427672961</v>
       </c>
       <c r="E4">
-        <v>0.6437659033078881</v>
+        <v>0.64376590330788808</v>
       </c>
       <c r="F4">
-        <v>0.7116736990154713</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>0.71167369901547128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -480,16 +508,16 @@
         <v>600</v>
       </c>
       <c r="D5">
-        <v>0.8338557993730408</v>
+        <v>0.83385579937304077</v>
       </c>
       <c r="E5">
-        <v>0.6768447837150128</v>
+        <v>0.67684478371501278</v>
       </c>
       <c r="F5">
         <v>0.7471910112359551</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -506,10 +534,10 @@
         <v>0.7048346055979644</v>
       </c>
       <c r="F6">
-        <v>0.7537414965986394</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>0.75374149659863943</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -520,13 +548,13 @@
         <v>600</v>
       </c>
       <c r="D7">
-        <v>0.8260869565217391</v>
+        <v>0.82608695652173914</v>
       </c>
       <c r="E7">
-        <v>0.7251908396946565</v>
+        <v>0.72519083969465647</v>
       </c>
       <c r="F7">
-        <v>0.7723577235772358</v>
+        <v>0.77235772357723576</v>
       </c>
     </row>
   </sheetData>

</xml_diff>